<commit_message>
Updating some xml and reports side of the project to adapt to jenkins.
</commit_message>
<xml_diff>
--- a/src/test/resources/uiTestData/ModulesOnHomePage.xlsx
+++ b/src/test/resources/uiTestData/ModulesOnHomePage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aslihancap/Desktop/Insiderone_UI_API_Automation/src/test/resources/uiTestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A6D81-9A43-524D-8A84-6DCFE3B58ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2884718-8D5B-A34A-BC9E-679789587508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="15540" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>